<commit_message>
hapus dan upload modul surat
</commit_message>
<xml_diff>
--- a/assets/excel/Data surat.xlsx
+++ b/assets/excel/Data surat.xlsx
@@ -362,7 +362,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,51 +496,6 @@
       <c r="B24"/>
       <c r="C24"/>
     </row>
-    <row r="25" spans="1:3">
-      <c r="A25"/>
-      <c r="B25"/>
-      <c r="C25"/>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26"/>
-      <c r="B26"/>
-      <c r="C26"/>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27"/>
-      <c r="B27"/>
-      <c r="C27"/>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28"/>
-      <c r="B28"/>
-      <c r="C28"/>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29"/>
-      <c r="B29"/>
-      <c r="C29"/>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30"/>
-      <c r="B30"/>
-      <c r="C30"/>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31"/>
-      <c r="B31"/>
-      <c r="C31"/>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32"/>
-      <c r="B32"/>
-      <c r="C32"/>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33"/>
-      <c r="B33"/>
-      <c r="C33"/>
-    </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>

</xml_diff>